<commit_message>
Save 19170 occurrence xlsx file
</commit_message>
<xml_diff>
--- a/typo_lookup.xlsx
+++ b/typo_lookup.xlsx
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">lookup!$B$1:$B$594</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -3772,7 +3772,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3786,7 +3786,7 @@
   <dimension ref="A1:B594"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>